<commit_message>
status complete not fix history not yet
</commit_message>
<xml_diff>
--- a/uploads/master/template_baju.xlsx
+++ b/uploads/master/template_baju.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deyelovi\Documents\JASAWEB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deyelovi\Documents\JASAWEB\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>NAMA BAJU</t>
   </si>
@@ -45,6 +45,18 @@
   </si>
   <si>
     <t>DETAIL</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>Deye Klambi</t>
+  </si>
+  <si>
+    <t>PINK</t>
+  </si>
+  <si>
+    <t>Deye gawe klambi</t>
   </si>
 </sst>
 </file>
@@ -391,24 +403,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="28" style="3" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" style="3" customWidth="1"/>
+    <col min="2" max="3" width="23.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28" style="3" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,19 +428,48 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="F2" s="4">
+        <v>3000000</v>
+      </c>
+      <c r="G2" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>